<commit_message>
add NaN, e, pi, Infinity to sbml-module expressions
</commit_message>
<xml_diff>
--- a/docs/export featured support.xlsx
+++ b/docs/export featured support.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>SLV</t>
   </si>
@@ -104,13 +104,25 @@
   </si>
   <si>
     <t>Mrgsolve/R</t>
+  </si>
+  <si>
+    <t>e, pi</t>
+  </si>
+  <si>
+    <t>Infinity</t>
+  </si>
+  <si>
+    <t>NaN</t>
+  </si>
+  <si>
+    <t>nthRoot</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -134,6 +146,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -196,7 +214,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -210,6 +228,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -619,10 +638,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J21"/>
+  <dimension ref="A1:J25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -914,6 +933,58 @@
       <c r="I21" s="5"/>
       <c r="J21" s="5"/>
     </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>30</v>
+      </c>
+      <c r="C22" s="9"/>
+      <c r="D22" s="9"/>
+      <c r="E22" s="9"/>
+      <c r="F22" s="9"/>
+      <c r="G22" s="9"/>
+      <c r="H22" s="9"/>
+      <c r="I22" s="9"/>
+      <c r="J22" s="9"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>31</v>
+      </c>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="5"/>
+      <c r="G23" s="5"/>
+      <c r="H23" s="5"/>
+      <c r="I23" s="5"/>
+      <c r="J23" s="5"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>32</v>
+      </c>
+      <c r="C24" s="5"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="5"/>
+      <c r="G24" s="5"/>
+      <c r="H24" s="5"/>
+      <c r="I24" s="5"/>
+      <c r="J24" s="5"/>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>33</v>
+      </c>
+      <c r="C25" s="5"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="5"/>
+      <c r="F25" s="5"/>
+      <c r="G25" s="5"/>
+      <c r="H25" s="5"/>
+      <c r="I25" s="5"/>
+      <c r="J25" s="5"/>
+    </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="C1:F1"/>
@@ -921,7 +992,7 @@
     <mergeCell ref="I1:J1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add support of INF in SBML values
</commit_message>
<xml_diff>
--- a/docs/export featured support.xlsx
+++ b/docs/export featured support.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>SLV</t>
   </si>
@@ -116,6 +116,9 @@
   </si>
   <si>
     <t>nthRoot</t>
+  </si>
+  <si>
+    <t>NaN, Infinity in const</t>
   </si>
 </sst>
 </file>
@@ -225,10 +228,10 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -638,9 +641,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J25"/>
+  <dimension ref="A1:J26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
       <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
@@ -657,20 +660,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8" t="s">
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8" t="s">
+      <c r="H1" s="9"/>
+      <c r="I1" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="J1" s="8"/>
+      <c r="J1" s="9"/>
     </row>
     <row r="2" spans="1:10" s="1" customFormat="1" ht="24.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C2" s="1" t="s">
@@ -937,14 +940,14 @@
       <c r="A22" t="s">
         <v>30</v>
       </c>
-      <c r="C22" s="9"/>
-      <c r="D22" s="9"/>
-      <c r="E22" s="9"/>
-      <c r="F22" s="9"/>
-      <c r="G22" s="9"/>
-      <c r="H22" s="9"/>
-      <c r="I22" s="9"/>
-      <c r="J22" s="9"/>
+      <c r="C22" s="8"/>
+      <c r="D22" s="8"/>
+      <c r="E22" s="8"/>
+      <c r="F22" s="8"/>
+      <c r="G22" s="8"/>
+      <c r="H22" s="8"/>
+      <c r="I22" s="8"/>
+      <c r="J22" s="8"/>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
@@ -984,6 +987,19 @@
       <c r="H25" s="5"/>
       <c r="I25" s="5"/>
       <c r="J25" s="5"/>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>34</v>
+      </c>
+      <c r="C26" s="5"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="5"/>
+      <c r="F26" s="5"/>
+      <c r="G26" s="5"/>
+      <c r="H26" s="5"/>
+      <c r="I26" s="5"/>
+      <c r="J26" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>